<commit_message>
CREATE second attempt of the model
</commit_message>
<xml_diff>
--- a/source_code/data/eb.xlsx
+++ b/source_code/data/eb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\district_thermal_energy_systems_with_power_markets\source_code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53803C63-F3B4-4F0B-B1ED-6F9EB85EE1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92A9608-266D-459B-82B0-0A9FAA6538C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,12 +41,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
   <si>
     <t>p_eb_eta</t>
   </si>
   <si>
     <t>p_eb_c_inv</t>
+  </si>
+  <si>
+    <t>p_eb_c_fix</t>
   </si>
 </sst>
 </file>
@@ -364,26 +367,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.99</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>110000</v>
+      </c>
+      <c r="C2">
+        <v>1110</v>
       </c>
     </row>
   </sheetData>
@@ -393,26 +402,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45690EF8-0787-4222-A3FE-ACB6CD2B8582}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.99</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>105000</v>
+      </c>
+      <c r="C2">
+        <v>1080</v>
       </c>
     </row>
   </sheetData>
@@ -422,26 +437,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E19C56-C44F-456C-9F61-25DA0654B4B1}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.99</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>103750</v>
+      </c>
+      <c r="C2">
+        <v>1058.0550000000001</v>
       </c>
     </row>
   </sheetData>
@@ -451,26 +472,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C08366A-A187-448F-95A9-2B811BDB695F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.99</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>102500</v>
+      </c>
+      <c r="C2">
+        <v>1031.47</v>
       </c>
     </row>
   </sheetData>
@@ -480,26 +507,32 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFFC2A3-5E73-48EB-A397-B717D9502D5A}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.99</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>101250</v>
+      </c>
+      <c r="C2">
+        <v>1004.885</v>
       </c>
     </row>
   </sheetData>
@@ -509,26 +542,32 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9672F23E-57C2-42EA-A960-2EB80F9B3C17}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.99</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>100000</v>
+      </c>
+      <c r="C2">
+        <v>978.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADAPT fix costs, cop for TTES and cop for HP (air) based on temperature
</commit_message>
<xml_diff>
--- a/source_code/data/eb.xlsx
+++ b/source_code/data/eb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\district_thermal_energy_systems_with_power_markets\source_code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92A9608-266D-459B-82B0-0A9FAA6538C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACF03C0-EFA2-4AC3-B9C7-E9D0EB61E113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,15 +41,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="2">
   <si>
     <t>p_eb_eta</t>
   </si>
   <si>
     <t>p_eb_c_inv</t>
-  </si>
-  <si>
-    <t>p_eb_c_fix</t>
   </si>
 </sst>
 </file>
@@ -367,32 +364,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.99</v>
       </c>
       <c r="B2">
         <v>110000</v>
-      </c>
-      <c r="C2">
-        <v>1110</v>
       </c>
     </row>
   </sheetData>
@@ -402,32 +393,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45690EF8-0787-4222-A3FE-ACB6CD2B8582}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.99</v>
       </c>
       <c r="B2">
         <v>105000</v>
-      </c>
-      <c r="C2">
-        <v>1080</v>
       </c>
     </row>
   </sheetData>
@@ -437,32 +422,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E19C56-C44F-456C-9F61-25DA0654B4B1}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.99</v>
       </c>
       <c r="B2">
         <v>103750</v>
-      </c>
-      <c r="C2">
-        <v>1058.0550000000001</v>
       </c>
     </row>
   </sheetData>
@@ -472,32 +451,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C08366A-A187-448F-95A9-2B811BDB695F}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.99</v>
       </c>
       <c r="B2">
         <v>102500</v>
-      </c>
-      <c r="C2">
-        <v>1031.47</v>
       </c>
     </row>
   </sheetData>
@@ -507,32 +480,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFFC2A3-5E73-48EB-A397-B717D9502D5A}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.99</v>
       </c>
       <c r="B2">
         <v>101250</v>
-      </c>
-      <c r="C2">
-        <v>1004.885</v>
       </c>
     </row>
   </sheetData>
@@ -542,32 +509,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9672F23E-57C2-42EA-A960-2EB80F9B3C17}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.99</v>
       </c>
       <c r="B2">
         <v>100000</v>
-      </c>
-      <c r="C2">
-        <v>978.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>